<commit_message>
Retune with delays correct
</commit_message>
<xml_diff>
--- a/micro.xlsx
+++ b/micro.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>Photon</t>
   </si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t>~0.9</t>
-  </si>
-  <si>
-    <t>~0.2</t>
   </si>
   <si>
     <t>Atmel SAMD21 32-bit ARM Cortex M0+</t>
@@ -509,7 +506,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -526,7 +523,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -547,7 +544,7 @@
         <v>7</v>
       </c>
       <c r="L1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -558,7 +555,7 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2">
         <v>120</v>
@@ -576,13 +573,13 @@
         <v>8</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
+        <v>38</v>
+      </c>
+      <c r="L2">
+        <v>0.2</v>
       </c>
       <c r="M2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -593,7 +590,7 @@
         <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3">
         <v>48</v>
@@ -611,7 +608,7 @@
         <v>8</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L3" t="s">
         <v>24</v>
@@ -622,7 +619,7 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>16</v>
@@ -639,8 +636,8 @@
       <c r="H4" t="s">
         <v>15</v>
       </c>
-      <c r="L4" t="s">
-        <v>25</v>
+      <c r="L4">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -651,7 +648,7 @@
         <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <v>48</v>
@@ -666,7 +663,7 @@
         <v>14</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L5" t="s">
         <v>24</v>
@@ -680,7 +677,7 @@
         <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6">
         <v>32</v>
@@ -709,13 +706,13 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7">
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>16</v>
@@ -730,18 +727,18 @@
         <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L7" t="s">
         <v>25</v>
       </c>
       <c r="M7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8">
         <v>16</v>
@@ -750,32 +747,32 @@
         <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10">
         <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10">
         <v>1200</v>
       </c>
       <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" t="s">
         <v>42</v>
-      </c>
-      <c r="I10" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>